<commit_message>
worked on recovery and started MBA project for V4 boards
</commit_message>
<xml_diff>
--- a/HYDRA_V4_RECOVERY/STM32H730_PINOUT.xlsx
+++ b/HYDRA_V4_RECOVERY/STM32H730_PINOUT.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_RECOVERY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E4F567-1685-4208-8C9A-B8CDBCC8F05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CCE83D-38CF-41C6-94F6-4D147DCDDFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="-21600" windowWidth="19200" windowHeight="21000" xr2:uid="{367BEAEE-6719-4EDD-BA6A-83B7D18C34CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{367BEAEE-6719-4EDD-BA6A-83B7D18C34CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="160">
   <si>
     <t>PE2</t>
   </si>
@@ -399,13 +400,130 @@
   </si>
   <si>
     <t>HYDRA_V4_RECOVERY</t>
+  </si>
+  <si>
+    <t>BUZZER</t>
+  </si>
+  <si>
+    <t>CAM_nPWRDN</t>
+  </si>
+  <si>
+    <t>CAM_nRST</t>
+  </si>
+  <si>
+    <t>IMU_nRST</t>
+  </si>
+  <si>
+    <t>IMU_ODR</t>
+  </si>
+  <si>
+    <t>CAM_D6</t>
+  </si>
+  <si>
+    <t>CAM_D7</t>
+  </si>
+  <si>
+    <t>CAM_D2</t>
+  </si>
+  <si>
+    <t>SD_D3</t>
+  </si>
+  <si>
+    <t>SD_D2</t>
+  </si>
+  <si>
+    <t>SD_CMD</t>
+  </si>
+  <si>
+    <t>SD_CK</t>
+  </si>
+  <si>
+    <t>CAM_D5</t>
+  </si>
+  <si>
+    <t>CAM_D4</t>
+  </si>
+  <si>
+    <t>CAM_D0</t>
+  </si>
+  <si>
+    <t>CAM_D1</t>
+  </si>
+  <si>
+    <t>CAM_D3</t>
+  </si>
+  <si>
+    <t>SD_D0</t>
+  </si>
+  <si>
+    <t>SD_D1</t>
+  </si>
+  <si>
+    <t>CAM_HSYNC</t>
+  </si>
+  <si>
+    <t>CAM_PIXCLK</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>VCC_V_SENSE</t>
+  </si>
+  <si>
+    <t>5V_V_SENSE</t>
+  </si>
+  <si>
+    <t>3V3_V_SENSE</t>
+  </si>
+  <si>
+    <t>PYRO_PWR_V_SENSE</t>
+  </si>
+  <si>
+    <t>DROGUE_V_SENSE</t>
+  </si>
+  <si>
+    <t>MAIN_V_SENSE</t>
+  </si>
+  <si>
+    <t>5V_IMON</t>
+  </si>
+  <si>
+    <t>3V3_IMON</t>
+  </si>
+  <si>
+    <t>DROGUE_I_SENSE</t>
+  </si>
+  <si>
+    <t>MAIN_I_SENSE</t>
+  </si>
+  <si>
+    <t>DROGUE_TRIG</t>
+  </si>
+  <si>
+    <t>MAIN_TRIG</t>
+  </si>
+  <si>
+    <t>POST_SW_PYRO_V_SENSE</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>MCU_R_LED</t>
+  </si>
+  <si>
+    <t>MCU_G_LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +531,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +548,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,9 +570,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,19 +909,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A805A7AA-E2D5-448E-8A3B-A198DD3D8A13}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -805,27 +937,39 @@
       <c r="E1" t="s">
         <v>109</v>
       </c>
+      <c r="F1" t="s">
+        <v>142</v>
+      </c>
       <c r="G1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -835,8 +979,11 @@
       <c r="E4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -846,8 +993,11 @@
       <c r="E5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
         <v>5</v>
@@ -858,8 +1008,11 @@
       <c r="E6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:A70" si="0">A6+1</f>
         <v>6</v>
@@ -867,80 +1020,107 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="G8" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="G9" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="G10" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="G11" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="G13" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="G14" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -948,8 +1128,17 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -960,8 +1149,14 @@
       <c r="D17" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -969,8 +1164,14 @@
       <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -978,35 +1179,53 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="F19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" t="s">
+        <v>143</v>
+      </c>
+      <c r="I19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="G20" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="G21" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G22" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1017,8 +1236,17 @@
       <c r="D23" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1026,8 +1254,17 @@
       <c r="B24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1035,8 +1272,17 @@
       <c r="B25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G25" t="s">
+        <v>143</v>
+      </c>
+      <c r="I25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1044,26 +1290,41 @@
       <c r="B26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="F26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G26" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="G27" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G28" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1074,8 +1335,17 @@
       <c r="E29" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" t="s">
+        <v>143</v>
+      </c>
+      <c r="I29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1083,8 +1353,17 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>143</v>
+      </c>
+      <c r="G30" t="s">
+        <v>143</v>
+      </c>
+      <c r="I30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1095,8 +1374,17 @@
       <c r="E31" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1104,8 +1392,17 @@
       <c r="B32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" t="s">
+        <v>143</v>
+      </c>
+      <c r="I32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1116,8 +1413,17 @@
       <c r="D33" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1125,8 +1431,17 @@
       <c r="B34" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F34" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1134,8 +1449,17 @@
       <c r="B35" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F35" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" t="s">
+        <v>143</v>
+      </c>
+      <c r="I35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1143,8 +1467,17 @@
       <c r="B36" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F36" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" t="s">
+        <v>143</v>
+      </c>
+      <c r="I36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1152,8 +1485,14 @@
       <c r="B37" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>143</v>
+      </c>
+      <c r="I37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1161,8 +1500,14 @@
       <c r="B38" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>143</v>
+      </c>
+      <c r="I38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1170,8 +1515,11 @@
       <c r="B39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1179,8 +1527,11 @@
       <c r="B40" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1188,8 +1539,11 @@
       <c r="B41" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1197,8 +1551,11 @@
       <c r="B42" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1206,8 +1563,11 @@
       <c r="B43" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1215,8 +1575,11 @@
       <c r="B44" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1224,8 +1587,11 @@
       <c r="B45" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1233,8 +1599,11 @@
       <c r="B46" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1242,8 +1611,11 @@
       <c r="B47" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1251,35 +1623,47 @@
       <c r="B48" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="G48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="G49" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="G50" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G51" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1287,8 +1671,11 @@
       <c r="B52" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1299,8 +1686,11 @@
       <c r="C53" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1311,8 +1701,14 @@
       <c r="D54" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>143</v>
+      </c>
+      <c r="I54" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1323,8 +1719,14 @@
       <c r="D55" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>143</v>
+      </c>
+      <c r="I55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1332,8 +1734,11 @@
       <c r="B56" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1341,8 +1746,11 @@
       <c r="B57" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1350,8 +1758,11 @@
       <c r="B58" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1359,8 +1770,11 @@
       <c r="B59" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1371,8 +1785,11 @@
       <c r="E60" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G60" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1383,8 +1800,11 @@
       <c r="E61" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G61" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1392,8 +1812,11 @@
       <c r="B62" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G62" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1401,8 +1824,11 @@
       <c r="B63" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1419,8 +1845,14 @@
       <c r="E64" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>143</v>
+      </c>
+      <c r="I64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1437,8 +1869,14 @@
       <c r="E65" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G65" t="s">
+        <v>143</v>
+      </c>
+      <c r="I65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1452,8 +1890,14 @@
       <c r="E66" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G66" t="s">
+        <v>143</v>
+      </c>
+      <c r="I66" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -1467,8 +1911,14 @@
       <c r="E67" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G67" t="s">
+        <v>143</v>
+      </c>
+      <c r="I67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -1476,8 +1926,11 @@
       <c r="B68" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G68" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -1488,8 +1941,11 @@
       <c r="E69" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -1500,8 +1956,11 @@
       <c r="E70" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G70" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" ref="A71:A101" si="1">A70+1</f>
         <v>70</v>
@@ -1509,8 +1968,11 @@
       <c r="B71" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G71" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1518,17 +1980,23 @@
       <c r="B72" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="G72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G73" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -1536,8 +2004,11 @@
       <c r="B74" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G74" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -1545,8 +2016,11 @@
       <c r="B75" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G75" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -1554,17 +2028,23 @@
       <c r="B76" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77">
+      <c r="G76" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G77" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -1572,8 +2052,11 @@
       <c r="B78" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G78" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -1587,8 +2070,11 @@
       <c r="E79" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G79" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -1602,8 +2088,14 @@
       <c r="E80" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G80" t="s">
+        <v>143</v>
+      </c>
+      <c r="I80" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -1617,8 +2109,11 @@
       <c r="E81" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G81" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -1626,8 +2121,11 @@
       <c r="B82" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G82" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -1635,8 +2133,14 @@
       <c r="B83" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G83" t="s">
+        <v>143</v>
+      </c>
+      <c r="I83" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -1650,8 +2154,14 @@
       <c r="E84" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G84" t="s">
+        <v>143</v>
+      </c>
+      <c r="I84" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -1662,8 +2172,14 @@
       <c r="E85" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G85" t="s">
+        <v>143</v>
+      </c>
+      <c r="I85" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -1671,8 +2187,11 @@
       <c r="B86" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G86" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -1680,8 +2199,11 @@
       <c r="B87" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G87" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -1695,8 +2217,14 @@
       <c r="E88" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G88" t="s">
+        <v>143</v>
+      </c>
+      <c r="I88" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -1707,8 +2235,14 @@
       <c r="D89" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G89" t="s">
+        <v>143</v>
+      </c>
+      <c r="I89" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -1719,8 +2253,14 @@
       <c r="D90" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G90" t="s">
+        <v>143</v>
+      </c>
+      <c r="I90" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -1731,8 +2271,14 @@
       <c r="D91" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G91" t="s">
+        <v>143</v>
+      </c>
+      <c r="I91" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -1743,8 +2289,14 @@
       <c r="E92" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G92" t="s">
+        <v>143</v>
+      </c>
+      <c r="I92" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -1755,8 +2307,14 @@
       <c r="E93" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G93" t="s">
+        <v>143</v>
+      </c>
+      <c r="I93" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -1767,17 +2325,20 @@
       <c r="E94" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95">
+      <c r="G94" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -1794,8 +2355,14 @@
       <c r="E96" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G96" t="s">
+        <v>143</v>
+      </c>
+      <c r="I96" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -1812,8 +2379,14 @@
       <c r="E97" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G97" t="s">
+        <v>143</v>
+      </c>
+      <c r="I97" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -1824,8 +2397,14 @@
       <c r="E98" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G98" t="s">
+        <v>143</v>
+      </c>
+      <c r="I98" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -1836,26 +2415,39 @@
       <c r="E99" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100">
+      <c r="G99" t="s">
+        <v>143</v>
+      </c>
+      <c r="I99" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101">
+      <c r="G100" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G101" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pretty much done development, good to start review. it's not perfect, but it needs to get ordered
</commit_message>
<xml_diff>
--- a/HYDRA_V4_RECOVERY/STM32H730_PINOUT.xlsx
+++ b/HYDRA_V4_RECOVERY/STM32H730_PINOUT.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_RECOVERY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\Documents\Projects\HYDRA\HYDRA_V4_RECOVERY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CCE83D-38CF-41C6-94F6-4D147DCDDFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DCC4CE-0008-4A67-A694-2C842D8244F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{367BEAEE-6719-4EDD-BA6A-83B7D18C34CB}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="16410" windowHeight="14505" xr2:uid="{367BEAEE-6719-4EDD-BA6A-83B7D18C34CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -570,11 +569,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,7 +910,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,15 +1022,15 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1279,7 +1277,7 @@
         <v>143</v>
       </c>
       <c r="I25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1297,7 +1295,7 @@
         <v>143</v>
       </c>
       <c r="I26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worked on homogenization, found issues with TCAN1146 implementation and need to figure out LINK
</commit_message>
<xml_diff>
--- a/HYDRA_V4_RECOVERY/STM32H730_PINOUT.xlsx
+++ b/HYDRA_V4_RECOVERY/STM32H730_PINOUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\Documents\Projects\HYDRA\HYDRA_V4_RECOVERY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_RECOVERY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DCC4CE-0008-4A67-A694-2C842D8244F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F60A74-811A-4556-8D51-3C9A3C7D71B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="16410" windowHeight="14505" xr2:uid="{367BEAEE-6719-4EDD-BA6A-83B7D18C34CB}"/>
+    <workbookView xWindow="1800" yWindow="1965" windowWidth="27000" windowHeight="14235" xr2:uid="{367BEAEE-6719-4EDD-BA6A-83B7D18C34CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="161">
   <si>
     <t>PE2</t>
   </si>
@@ -516,6 +516,9 @@
   </si>
   <si>
     <t>MCU_G_LED</t>
+  </si>
+  <si>
+    <t>CAM_nINTRQ</t>
   </si>
 </sst>
 </file>
@@ -909,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A805A7AA-E2D5-448E-8A3B-A198DD3D8A13}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,6 +1960,9 @@
       <c r="G70" t="s">
         <v>143</v>
       </c>
+      <c r="I70" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">

</xml_diff>